<commit_message>
Committing final code for Job description page
</commit_message>
<xml_diff>
--- a/Tests/linkedIn_login_data.xlsx
+++ b/Tests/linkedIn_login_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git work\CCWebsiteAutomation\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git work\CCWebsiteAutomationWithPython\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84555F84-0B95-4EB1-B1EC-8FA22261EDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F729E377-0725-4E33-9B95-B974424A060B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{27B27FC4-87B9-473B-B86A-890554AC6FA3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>fedcre@t!ve</t>
+  </si>
+  <si>
+    <t>saamaajik.fed.cci@gmail.com</t>
+  </si>
+  <si>
+    <t>S0c!al@2022</t>
   </si>
 </sst>
 </file>
@@ -426,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BADA0E25-C6B8-4C93-A9C8-3B0F1B01D29A}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,10 +460,24 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{287E17A9-523A-4692-A826-CD5CCA79538C}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{277C4F3E-2405-4FEC-8C26-4D849000B893}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{D8E5384E-8935-44B3-A91F-A71752557403}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{0322916A-E055-4683-A719-1AF481B3ACE0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>